<commit_message>
Committed Corporate Customer excel file
</commit_message>
<xml_diff>
--- a/Data/BackDatedTermDepositsFCY.xlsx
+++ b/Data/BackDatedTermDepositsFCY.xlsx
@@ -12,12 +12,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Transaction Number</t>
   </si>
   <si>
     <t>MM2300400080</t>
+  </si>
+  <si>
+    <t>MM2316800125</t>
+  </si>
+  <si>
+    <t>MM2316800147</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -78,6 +84,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>